<commit_message>
Fixed true perlin noise
</commit_message>
<xml_diff>
--- a/perlin_terrain_parameters.xlsx
+++ b/perlin_terrain_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\College\Grad\Spring 2025\CS6366 - Computer Graphics\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E3C0CC-8DE1-41F9-A6C5-00454C56E860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF794D54-AB3B-4F71-9B21-2C7C3E7A274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25560" yWindow="19320" windowWidth="31935" windowHeight="12345" xr2:uid="{90AE6792-0FDF-464B-AB68-E2803D786D7A}"/>
+    <workbookView xWindow="28110" yWindow="24585" windowWidth="28770" windowHeight="11100" xr2:uid="{90AE6792-0FDF-464B-AB68-E2803D786D7A}"/>
   </bookViews>
   <sheets>
     <sheet name="fractal" sheetId="1" r:id="rId1"/>
@@ -386,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -396,7 +396,6 @@
       </extLst>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187CAB77-9958-46D5-B6A2-E44291D87BF8}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1214,7 +1213,7 @@
       <c r="C27" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27">
         <v>4</v>
       </c>
       <c r="E27">

</xml_diff>

<commit_message>
Testing different parameter values for fractal perlin noise
</commit_message>
<xml_diff>
--- a/perlin_terrain_parameters.xlsx
+++ b/perlin_terrain_parameters.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\College\Grad\Spring 2025\CS6366 - Computer Graphics\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF794D54-AB3B-4F71-9B21-2C7C3E7A274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BDC26C-9868-49EB-95B3-D9B5CE4D6E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28110" yWindow="24585" windowWidth="28770" windowHeight="11100" xr2:uid="{90AE6792-0FDF-464B-AB68-E2803D786D7A}"/>
+    <workbookView xWindow="28110" yWindow="12045" windowWidth="28770" windowHeight="19635" activeTab="2" xr2:uid="{90AE6792-0FDF-464B-AB68-E2803D786D7A}"/>
   </bookViews>
   <sheets>
     <sheet name="fractal" sheetId="1" r:id="rId1"/>
     <sheet name="gaussian" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="118">
   <si>
     <t>Terrain Type</t>
   </si>
@@ -352,6 +353,45 @@
   </si>
   <si>
     <t>Deep pit close to high peaks. Could be used to simulate mountainous environments with a lake in the pit</t>
+  </si>
+  <si>
+    <t>octaves</t>
+  </si>
+  <si>
+    <t>persistence</t>
+  </si>
+  <si>
+    <t>amplitude</t>
+  </si>
+  <si>
+    <t>lacunarity</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>most smooth</t>
+  </si>
+  <si>
+    <t>Good example of very smoothed terrain</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Good mountain range example</t>
+  </si>
+  <si>
+    <t>Good example of one mountain and one lake</t>
   </si>
 </sst>
 </file>
@@ -449,6 +489,21 @@
     </a>
   </bag>
 </FeaturePropertyBags>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{23DB44EF-9BC2-41A5-A062-092038025344}" name="Table1" displayName="Table1" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41" xr:uid="{23DB44EF-9BC2-41A5-A062-092038025344}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E0486653-9FE8-4D3C-9050-08B467859AA8}" name="octaves"/>
+    <tableColumn id="2" xr3:uid="{815BA72F-9818-4CD2-98C2-B61D9F35B9E3}" name="persistence"/>
+    <tableColumn id="3" xr3:uid="{46425A37-9216-495D-BF7D-A46D8B4AE943}" name="amplitude"/>
+    <tableColumn id="4" xr3:uid="{C6904CCC-C280-4901-9E67-230B62C10A9E}" name="lacunarity"/>
+    <tableColumn id="5" xr3:uid="{5F824CDF-5F92-4B2D-ADEC-93D1520D954A}" name="scale"/>
+    <tableColumn id="6" xr3:uid="{915C1E13-38E0-4188-9A42-DC96E06838AB}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187CAB77-9958-46D5-B6A2-E44291D87BF8}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1503,4 +1558,771 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0861267F-4C6D-4F22-BF66-52B16868DF1D}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.75</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.75</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0.75</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>200</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.75</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.75</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.75</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.75</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.75</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>200</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1.5</v>
+      </c>
+      <c r="C14">
+        <v>0.75</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <v>0.75</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+      <c r="E15">
+        <v>200</v>
+      </c>
+      <c r="F15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.75</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>200</v>
+      </c>
+      <c r="F16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>1.5</v>
+      </c>
+      <c r="C17">
+        <v>0.75</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>200</v>
+      </c>
+      <c r="F17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.25</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0.75</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0.25</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+      <c r="E22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+      <c r="E23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.75</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+      <c r="E24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+      <c r="E25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0.25</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+      <c r="E26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+      <c r="E27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.75</v>
+      </c>
+      <c r="D28">
+        <v>0.5</v>
+      </c>
+      <c r="E28">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="E29">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.25</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.75</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.5</v>
+      </c>
+      <c r="E33">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>0.25</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+      <c r="E34">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>0.5</v>
+      </c>
+      <c r="D35">
+        <v>0.5</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0.75</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.5</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>0.25</v>
+      </c>
+      <c r="D38">
+        <v>0.5</v>
+      </c>
+      <c r="E38">
+        <v>500</v>
+      </c>
+      <c r="F38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>0.5</v>
+      </c>
+      <c r="D39">
+        <v>0.5</v>
+      </c>
+      <c r="E39">
+        <v>500</v>
+      </c>
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>0.75</v>
+      </c>
+      <c r="D40">
+        <v>0.5</v>
+      </c>
+      <c r="E40">
+        <v>500</v>
+      </c>
+      <c r="F40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0.5</v>
+      </c>
+      <c r="E41">
+        <v>500</v>
+      </c>
+      <c r="F41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>